<commit_message>
Update: fixed tray icon fallback and PyInstaller compatibility
</commit_message>
<xml_diff>
--- a/govt_jobs.xlsx
+++ b/govt_jobs.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G13" sqref="A2:G13"/>
@@ -505,6 +505,195 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2025-09-26 12:03</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Test Government Job - Software Engineer</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>https://example.com/test-job</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Not Applied</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2025-09-26 12:03</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>⚫Advertisement No.37/2025⚫Advertisement No.36/2025⚫Advertisement No.35/2025</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>https://www.ppsc.gop.pk/Adds/Advt No-37-2025 26-09-2025  X7 Version.pdf</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>PPSC</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Not Applied</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2025-09-26 17:44</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Test Government Job - Software Engineer</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>https://example.com/test-job</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Not Applied</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2025-09-26 17:45</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>⚫Advertisement No.37/2025⚫Advertisement No.36/2025⚫Advertisement No.35/2025</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>https://www.ppsc.gop.pk/Adds/Advt No-37-2025 26-09-2025  X7 Version.pdf</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>PPSC</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Not Applied</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2025-09-26 17:45</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Test Government Job - Software Engineer</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>https://example.com/test-job</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Not Applied</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2025-09-26 17:45</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>⚫Advertisement No.37/2025⚫Advertisement No.36/2025⚫Advertisement No.35/2025</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>https://www.ppsc.gop.pk/Adds/Advt No-37-2025 26-09-2025  X7 Version.pdf</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>PPSC</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Not Applied</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2025-09-28 21:09</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>⚫Advertisement No.37/2025⚫Advertisement No.36/2025⚫Advertisement No.35/2025</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>https://www.ppsc.gop.pk/Adds/Advt No-37-2025 26-09-2025  X7 Version.pdf</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>PPSC</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Not Applied</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>